<commit_message>
Windows. Video 168 Terminado. Instalación de Postgresql
</commit_message>
<xml_diff>
--- a/Python-Django.xlsx
+++ b/Python-Django.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Udemy\Python-Django\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701E0ACE-9424-49C1-B49F-4E56D389AC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F923D306-2BB5-4B0D-B2DD-C40BA72B2812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2922989A-4758-4A55-B984-BFE493B5C2EC}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{2922989A-4758-4A55-B984-BFE493B5C2EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Instrucciones" sheetId="1" r:id="rId1"/>
+    <sheet name="Postgresql" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>@classmethod</t>
   </si>
@@ -46,6 +47,15 @@
   </si>
   <si>
     <t>Abre un archivo y lo cierra al terminar de ejecutar esta instrucción, porque las instrucciones van contenidas. Con with se pueden llamar clases y se ejecutan automáticamente los métodos __enter__ y __exit__</t>
+  </si>
+  <si>
+    <t>Puerto</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -408,7 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D51C39B-C241-4E3E-A88B-95271DF767CA}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -437,4 +447,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCE6C4A-FC3A-4ADF-8668-1074E3047EB6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>5432</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>